<commit_message>
PROS-13075 - CCRU - POS 2020 KPIs - SAND Deployment
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2020/Benchmark 2020.xlsx
+++ b/Projects/CCRU/Data/KPIs_2020/Benchmark 2020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hyper" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="75">
   <si>
     <t xml:space="preserve">KPI Code</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">Values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERROR</t>
   </si>
   <si>
     <t xml:space="preserve">STANDARD 1</t>
@@ -137,12 +134,8 @@
 Juice Display 1st,
 Juice Display 2d,
 Mixability Display,
-Energy Display,
 Tea-Rich Display,
 Juice Display 1st</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy Display(PoS 2020 - MT Hypermarket - CAP, PoS 2020 - MT Hypermarket - REG, PoS 2020 - MT Hypermarket - NKA)</t>
   </si>
   <si>
     <t xml:space="preserve">STANDARD 22</t>
@@ -211,9 +204,10 @@
 Juice Display 1st</t>
   </si>
   <si>
-    <t xml:space="preserve">Cooler: Prime Position
-Cooler: w/o other products(PoS 2020 - MT ConvSmall - CAP, PoS 2020 - MT ConvSmall - REG, PoS 2020 - MT ConvSmall - NKA),
-Cooler: Merch Priority STD(PoS 2020 - MT ConvSmall - CAP, PoS 2020 - MT ConvSmall - REG, PoS 2020 - MT ConvSmall - NKA)</t>
+    <t xml:space="preserve">Cooler: Max 15,
+Cooler: Merch Priority STD,
+Cooler: Prime Position,
+Cooler: w/o other products</t>
   </si>
   <si>
     <t xml:space="preserve">Juice (JNSD) Availability,
@@ -269,14 +263,6 @@
     <t xml:space="preserve">Combo, 
 Combo: Other, 
 Combo2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combo, 
-Combo: Other, 
-Combo2(PoS 2020 - IC Cinema)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tea Availability(PoS 2020 - IC QSR - GastroMarket)</t>
   </si>
   <si>
     <t xml:space="preserve">Combo1, 
@@ -285,12 +271,6 @@
 Assortment Reminder</t>
   </si>
   <si>
-    <t xml:space="preserve">Combo1, 
-Combo2, 
-Combo3, 
-Assortment Reminder(PoS 2020 - IC QSR - FoodCourt, PoS 2020 - IC QSR - Classic, PoS 2020 - IC QSR - GastroMarket)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cooler: w/o other products,
 Cooler: Max 26</t>
   </si>
@@ -303,10 +283,6 @@
   <si>
     <t xml:space="preserve">Combo, 
 Combo Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combo, 
-Combo Other(PoS 2020 - IC Petrol - Medium, PoS 2020 - IC Petrol - Large)</t>
   </si>
   <si>
     <t xml:space="preserve">Impulse Activation,
@@ -338,31 +314,13 @@
 Cooler: w/o FC packs</t>
   </si>
   <si>
-    <t xml:space="preserve">Energy Availability(PoS 2020 - FT S - Bread, PoS 2020 - FT S - Dairy, PoS 2020 - FT S - Meat, PoS 2020 - FT S - Sweets, PoS 2020 - FT S - Veggies),
-Juice (JNSD) Availability(PoS 2020 - FT S - Beer, PoS 2020 - FT S - Tobacco),
-Water Availability(PoS 2020 - FT S - Beer),
-Tea Availability(PoS 2020 - FT S - Beer, PoS 2020 - FT S - Bread, PoS 2020 - FT S - Dairy, PoS 2020 - FT S - Tobacco)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Juice Display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juice Display(PoS 2020 - FT S - Beer, PoS 2020 - FT S - Bread, PoS 2020 - FT S - Dairy, PoS 2020 - FT S - Meat, PoS 2020 - FT S - Sweets, PoS 2020 - FT S - Tobacco, PoS 2020 - FT S - Veggies)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cooler: Doors(PoS 2020 - FT S - Dairy, PoS 2020 - FT S - Sweets, PoS 2020 - FT S - Veggies)</t>
   </si>
   <si>
     <t xml:space="preserve">Cooler: Prime Position,
 Cooler: Max 26,
 Cooler: Merch Priorty STD,
 Cooler: w/o FC products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cooler: Prime Position(PoS 2020 - FT S - Beer, PoS 2020 - FT S - Bread, PoS 2020 - FT S - Dairy, PoS 2020 - FT S - Meat, PoS 2020 - FT S - Sweets, PoS 2020 - FT S - Tobacco, PoS 2020 - FT S - Veggies),
-Cooler: Max 26(PoS 2020 - FT S - Beer, PoS 2020 - FT S - Bread, PoS 2020 - FT S - Dairy, PoS 2020 - FT S - Meat, PoS 2020 - FT S - Sweets, PoS 2020 - FT S - Tobacco, PoS 2020 - FT S - Veggies),
-Cooler: Merch Priorty STD(PoS 2020 - FT S - Dairy, PoS 2020 - FT S - Sweets, PoS 2020 - FT S - Veggies),
-Cooler: w/o FC products(PoS 2020 - FT S - Beer, PoS 2020 - FT S - Bread, PoS 2020 - FT S - Dairy, PoS 2020 - FT S - Meat, PoS 2020 - FT S - Sweets, PoS 2020 - FT S - Tobacco, PoS 2020 - FT S - Veggies)</t>
   </si>
 </sst>
 </file>
@@ -483,24 +441,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.1983805668016"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7651821862348"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="108.777327935223"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1943319838057"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0607287449393"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="17.1943319838057"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,164 +470,158 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="B6" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>20</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="B7" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="B8" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B9" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="B10" s="0" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>33</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -692,24 +640,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.79757085020243"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8218623481781"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="105.234817813765"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.36842105263158"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6518218623482"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -725,116 +672,107 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -853,24 +791,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.79757085020243"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8218623481781"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.45344129554656"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.36842105263158"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6518218623482"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -886,76 +823,73 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -974,24 +908,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.79757085020243"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8218623481781"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.9271255060729"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.36842105263158"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6518218623482"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1007,198 +940,192 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.18889</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.18889</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.18889</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.18889</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="B6" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>20</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1.18889</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1.18889</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1.18889</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1.18889</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1.18889</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1.18889</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1.18889</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1217,24 +1144,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.82591093117409"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8218623481781"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.45344129554656"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5101214574899"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6518218623482"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1250,93 +1176,90 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.111111</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.111111</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.111111</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.111111</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1.111111</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1355,24 +1278,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.82591093117409"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8218623481781"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.45344129554656"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5101214574899"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6518218623482"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1388,93 +1310,90 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.111111</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.111111</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.111111</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.111111</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1.111111</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1493,24 +1412,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.82591093117409"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9068825910931"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.45344129554656"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5101214574899"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1526,93 +1444,90 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.176471</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.176471</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.176471</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.176471</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1.176471</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1631,24 +1546,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.8582995951417"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9068825910931"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="177.331983805668"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.08502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1664,105 +1578,90 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1781,24 +1680,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.1983805668016"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7651821862348"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.45344129554656"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1814,161 +1712,158 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="B6" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>20</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="B7" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="B8" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B9" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1.1976048</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1987,24 +1882,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.82591093117409"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.4817813765182"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.45344129554656"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5101214574899"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2020,178 +1914,175 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B9" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2210,24 +2101,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.82591093117409"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.4817813765182"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.45344129554656"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5101214574899"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2243,178 +2133,175 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B9" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2433,24 +2320,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.82591093117409"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.4817813765182"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="113.574898785425"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5101214574899"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2466,181 +2352,175 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B9" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1.123596</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2659,24 +2539,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.6194331983806"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.82591093117409"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0202429149798"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.45344129554656"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.2753036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5101214574899"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.1943319838057"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2692,76 +2571,73 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.200048</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.200048</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.200048</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.200048</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2780,24 +2656,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="72.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.82591093117409"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.45344129554656"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5101214574899"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.9352226720648"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2813,93 +2688,90 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.200048</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.200048</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.200048</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.200048</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1.200048</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2918,24 +2790,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.79757085020243"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8218623481781"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.45344129554656"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.36842105263158"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6518218623482"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2951,110 +2822,107 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3073,24 +2941,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.79757085020243"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8218623481781"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4777327935223"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.36842105263158"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2550607287449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6518218623482"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3106,113 +2973,107 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1.38889</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>